<commit_message>
Creating, Listing and Changing Sheets
</commit_message>
<xml_diff>
--- a/my_file/Grades.xlsx
+++ b/my_file/Grades.xlsx
@@ -5,15 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lightrao/Desktop/LightTechZen/codeWithLight/youtube/TechWithTim/高效办公 用Python轻松操作Excel/automate-excel-with-python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lightrao/Desktop/LightTechZen/codeWithLight/youtube/TechWithTim/高效办公 用Python轻松操作Excel/automate-excel-with-python/my_file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8DBD2F-E677-ED49-8CA9-1B6079121107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74212211-10F5-2C43-B1EA-F58651609389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grades" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -423,7 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -554,4 +557,43 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB6C3FF-E918-0C47-B1B9-D2E0FBE2B082}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6850D5-D66A-644F-B05F-A673DF7FC0DE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A6CBAF3-52B6-DA4C-B1A1-2BE6C56287B3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>